<commit_message>
edit trial code spreadsheet
</commit_message>
<xml_diff>
--- a/trialcode_structure_meg.xlsx
+++ b/trialcode_structure_meg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kumarr13/Desktop/codereview/meg_codereview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8927608D-5AA9-C048-8F4A-E3041AAB9B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51E626E-BC70-8D41-AA44-8B1156F4F7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6180" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{F106D9C2-CD24-884D-84A5-CE5969B31AA3}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>Viewpoint</t>
   </si>
   <si>
-    <t>Expression Decoding</t>
-  </si>
-  <si>
     <t>angry</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>surprised</t>
   </si>
   <si>
-    <t xml:space="preserve">Identity Decoding </t>
-  </si>
-  <si>
     <t>AF01</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t>AM31</t>
   </si>
   <si>
-    <t>Viewpoint decoding</t>
-  </si>
-  <si>
     <t>FL</t>
   </si>
   <si>
@@ -116,6 +107,15 @@
   </si>
   <si>
     <t>full right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viewpoint </t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:T126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,13 +490,13 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -516,22 +516,22 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -552,22 +552,22 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -588,22 +588,22 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K4">
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -624,22 +624,22 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K5">
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -660,22 +660,22 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K6">
         <v>5</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>